<commit_message>
Updated some graphs and charts
</commit_message>
<xml_diff>
--- a/ModelsData/RainData/sanjuan.xlsx
+++ b/ModelsData/RainData/sanjuan.xlsx
@@ -20442,10 +20442,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1144"/>
+  <dimension ref="A1:N1144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H27"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20453,7 +20453,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>38129</v>
       </c>
@@ -20463,8 +20463,23 @@
       <c r="C1">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <v>3</v>
+      </c>
+      <c r="N1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>38129</v>
       </c>
@@ -20474,8 +20489,28 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>QUARTILE($C$1:$C$1144,J1)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:N2" si="0">QUARTILE($C$1:$C$1144,K1)</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>38129</v>
       </c>
@@ -20486,7 +20521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>38129</v>
       </c>
@@ -20510,7 +20545,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>38129</v>
       </c>
@@ -20535,7 +20570,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>38129</v>
       </c>
@@ -20546,21 +20581,21 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E27" si="0">E5+1</f>
+        <f t="shared" ref="E6:E27" si="1">E5+1</f>
         <v>3</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" ref="G6:G27" si="1">G5</f>
+        <f t="shared" ref="G6:G27" si="2">G5</f>
         <v>O1</v>
       </c>
       <c r="H6">
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>38129</v>
       </c>
@@ -20571,21 +20606,21 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H7">
         <v>0.09</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>38129</v>
       </c>
@@ -20596,21 +20631,21 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H8">
         <v>0.09</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>38129</v>
       </c>
@@ -20621,21 +20656,21 @@
         <v>0.02</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H9">
         <v>0.09</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>38129</v>
       </c>
@@ -20646,21 +20681,21 @@
         <v>0.06</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H10">
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>38129</v>
       </c>
@@ -20671,21 +20706,21 @@
         <v>0.03</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H11">
         <v>0.09</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>38130</v>
       </c>
@@ -20696,21 +20731,21 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H12">
         <v>0.09</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>38130</v>
       </c>
@@ -20721,21 +20756,21 @@
         <v>0.12</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H13">
         <v>0.09</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>38130</v>
       </c>
@@ -20746,21 +20781,21 @@
         <v>0.03</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H14">
         <v>0.09</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>38130</v>
       </c>
@@ -20771,21 +20806,21 @@
         <v>0.01</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H15">
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>38130</v>
       </c>
@@ -20796,14 +20831,14 @@
         <v>0.03</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H16">
@@ -20821,14 +20856,14 @@
         <v>0.01</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H17">
@@ -20846,14 +20881,14 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H18">
@@ -20871,14 +20906,14 @@
         <v>0.02</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H19">
@@ -20896,14 +20931,14 @@
         <v>0.34</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H20">
@@ -20921,14 +20956,14 @@
         <v>0.01</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H21">
@@ -20946,14 +20981,14 @@
         <v>0.1</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H22">
@@ -20971,14 +21006,14 @@
         <v>0.76</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H23">
@@ -20996,14 +21031,14 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H24">
@@ -21021,14 +21056,14 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H25">
@@ -21046,14 +21081,14 @@
         <v>0.3</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H26">
@@ -21071,14 +21106,14 @@
         <v>0.12</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>O1</v>
       </c>
       <c r="H27">

</xml_diff>